<commit_message>
Updated to reflect changes in set_parameters in model.py
</commit_message>
<xml_diff>
--- a/xls/data_input_4.xlsx
+++ b/xls/data_input_4.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="150">
   <si>
     <t>best</t>
   </si>
@@ -491,6 +491,45 @@
   </si>
   <si>
     <t>program_prop_nonsuccessoutcomes_death</t>
+  </si>
+  <si>
+    <t>epi_proportion_cases</t>
+  </si>
+  <si>
+    <t>tb_multiplier_force_smearneg</t>
+  </si>
+  <si>
+    <t>tb_proportion_early_progression</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_early_latent</t>
+  </si>
+  <si>
+    <t>tb_proportion_casefatality_untreated_smearpos</t>
+  </si>
+  <si>
+    <t>tb_proportion_casefatality_untreated_smearneg</t>
+  </si>
+  <si>
+    <t>tb_multiplier_bcg_protection</t>
+  </si>
+  <si>
+    <t>program_prop_vac</t>
+  </si>
+  <si>
+    <t>program_prop_unvac</t>
+  </si>
+  <si>
+    <t>program_rate_start_treatment</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_ds</t>
+  </si>
+  <si>
+    <t>program_prop_lowquality</t>
+  </si>
+  <si>
+    <t>program_rate_leavelowquality</t>
   </si>
 </sst>
 </file>
@@ -3269,10 +3308,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3357,7 +3396,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="71" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="C8" s="73">
         <v>1</v>
@@ -3367,497 +3406,618 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="71" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="C10" s="73">
-        <v>1</v>
+        <v>0.24</v>
       </c>
       <c r="D10" s="70"/>
       <c r="E10" s="70"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="73">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="71" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="73">
-        <v>7.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="70"/>
       <c r="E12" s="70"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="71" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="73">
-        <v>0.4</v>
+        <v>12</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C14" s="73">
-        <v>4</v>
+        <v>0.12</v>
       </c>
       <c r="D14" s="70"/>
       <c r="E14" s="70"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="71" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="C15" s="73">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="71" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C16" s="73">
-        <v>0.9</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="71" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C17" s="73">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="71" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C18" s="73">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="D18" s="70"/>
       <c r="E18" s="70"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="71" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C19" s="73">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="71" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C20" s="73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="70"/>
       <c r="E20" s="70"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="73">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="73">
+        <v>0.88</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="73">
+        <f>1-C22</f>
+        <v>0.12</v>
+      </c>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="73">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="73">
+        <v>0.9</v>
+      </c>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="73">
+        <v>26</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="73">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="73">
+        <v>2</v>
+      </c>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="73">
+        <v>3</v>
+      </c>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="73">
+        <v>3</v>
+      </c>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="73">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="73">
+      <c r="C32" s="73">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="71" t="s">
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="73">
+      <c r="C33" s="73">
         <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="71" t="s">
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="73">
-        <v>1.9</v>
-      </c>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="71" t="s">
+      <c r="C34" s="73">
+        <v>2</v>
+      </c>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="73">
+      <c r="C35" s="73">
         <v>0.9</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="71" t="s">
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="73">
+      <c r="C36" s="73">
         <v>0.6</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="71" t="s">
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="73">
+      <c r="C37" s="73">
         <v>0.4</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="71" t="s">
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="73">
-        <v>0.3</v>
-      </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="71" t="s">
+      <c r="C38" s="73">
+        <v>0.25</v>
+      </c>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="73">
+      <c r="C39" s="73">
         <v>4</v>
       </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="71" t="s">
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="73">
+      <c r="C40" s="73">
         <f>1/15</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="73">
-        <v>1960</v>
-      </c>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="73">
-        <v>2050</v>
-      </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="71" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="73">
-        <v>1950</v>
-      </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="73">
-        <v>0.2</v>
-      </c>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="71" t="s">
-        <v>131</v>
-      </c>
-      <c r="C34" s="73">
-        <v>1995</v>
-      </c>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="73">
-        <v>0.5</v>
-      </c>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="71" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" s="73">
-        <v>2010</v>
-      </c>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="73">
-        <v>0.2</v>
-      </c>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="73">
-        <v>0.6</v>
-      </c>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" s="73">
-        <v>0.4</v>
-      </c>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="71" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" s="73">
-        <v>0.25</v>
-      </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="73">
+        <v>1950</v>
+      </c>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="73">
+        <v>2050</v>
+      </c>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="73">
+        <v>1940</v>
+      </c>
+      <c r="D43" s="70"/>
+      <c r="E43" s="70"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="73">
+        <v>1990</v>
+      </c>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="73">
+        <v>2010</v>
+      </c>
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="73">
+        <v>0</v>
+      </c>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="73">
+        <v>0.85</v>
+      </c>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="71" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="73">
+        <v>0.6</v>
+      </c>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="73">
+        <v>0.4</v>
+      </c>
+      <c r="D49" s="70"/>
+      <c r="E49" s="70"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" s="73">
+        <v>0.4</v>
+      </c>
+      <c r="D50" s="70"/>
+      <c r="E50" s="70"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="73">
+        <v>2</v>
+      </c>
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="73">
+        <v>0.25</v>
+      </c>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="3" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="71" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="72">
+      <c r="C56" s="72">
         <v>20000000</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="4">
-        <v>0</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="4">
-        <v>3</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="4">
-        <v>0</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="6">
-        <v>0.4</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="6">
-        <v>0.1</v>
+        <v>5</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="6">
-        <v>0.3</v>
+        <v>6</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="6">
-        <v>0.5</v>
+      <c r="B59" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="4">
+        <v>3</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C63" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>